<commit_message>
added host age unit field
</commit_message>
<xml_diff>
--- a/template/canada_covid19/exampleInput/validTestData.xlsx
+++ b/template/canada_covid19/exampleInput/validTestData.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DG7"/>
+  <dimension ref="A1:DH7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -544,11 +544,11 @@
         <v/>
       </c>
       <c r="BC1" t="str">
+        <v/>
+      </c>
+      <c r="BD1" t="str">
         <v>Host exposure information</v>
       </c>
-      <c r="BD1" t="str">
-        <v/>
-      </c>
       <c r="BE1" t="str">
         <v/>
       </c>
@@ -580,11 +580,11 @@
         <v/>
       </c>
       <c r="BO1" t="str">
+        <v/>
+      </c>
+      <c r="BP1" t="str">
         <v>Sequencing</v>
       </c>
-      <c r="BP1" t="str">
-        <v/>
-      </c>
       <c r="BQ1" t="str">
         <v/>
       </c>
@@ -613,11 +613,11 @@
         <v/>
       </c>
       <c r="BZ1" t="str">
+        <v/>
+      </c>
+      <c r="CA1" t="str">
         <v>Bioinformatics and QC metrics</v>
       </c>
-      <c r="CA1" t="str">
-        <v/>
-      </c>
       <c r="CB1" t="str">
         <v/>
       </c>
@@ -691,11 +691,11 @@
         <v/>
       </c>
       <c r="CZ1" t="str">
+        <v/>
+      </c>
+      <c r="DA1" t="str">
         <v>Pathogen diagnostic testing</v>
       </c>
-      <c r="DA1" t="str">
-        <v/>
-      </c>
       <c r="DB1" t="str">
         <v/>
       </c>
@@ -709,9 +709,12 @@
         <v/>
       </c>
       <c r="DF1" t="str">
+        <v/>
+      </c>
+      <c r="DG1" t="str">
         <v>Contributor acknowledgement</v>
       </c>
-      <c r="DG1" t="str">
+      <c r="DH1" t="str">
         <v/>
       </c>
     </row>
@@ -855,198 +858,201 @@
         <v>host age</v>
       </c>
       <c r="AU2" t="str">
+        <v>host age unit</v>
+      </c>
+      <c r="AV2" t="str">
         <v>host age bin</v>
       </c>
-      <c r="AV2" t="str">
+      <c r="AW2" t="str">
         <v>host gender</v>
       </c>
-      <c r="AW2" t="str">
+      <c r="AX2" t="str">
         <v>host origin geo_loc name (country)</v>
       </c>
-      <c r="AX2" t="str">
+      <c r="AY2" t="str">
         <v>host subject ID</v>
       </c>
-      <c r="AY2" t="str">
+      <c r="AZ2" t="str">
         <v>symptom onset date</v>
       </c>
-      <c r="AZ2" t="str">
+      <c r="BA2" t="str">
         <v>signs and symptoms</v>
       </c>
-      <c r="BA2" t="str">
+      <c r="BB2" t="str">
         <v>pre-existing conditions and risk factors</v>
       </c>
-      <c r="BB2" t="str">
+      <c r="BC2" t="str">
         <v>complications</v>
       </c>
-      <c r="BC2" t="str">
+      <c r="BD2" t="str">
         <v>location of exposure geo_loc name (country)</v>
       </c>
-      <c r="BD2" t="str">
+      <c r="BE2" t="str">
         <v>destination of most recent travel (city)</v>
       </c>
-      <c r="BE2" t="str">
+      <c r="BF2" t="str">
         <v>destination of most recent travel (state/province/territory)</v>
       </c>
-      <c r="BF2" t="str">
+      <c r="BG2" t="str">
         <v>destination of most recent travel (country)</v>
       </c>
-      <c r="BG2" t="str">
+      <c r="BH2" t="str">
         <v>most recent travel departure date</v>
       </c>
-      <c r="BH2" t="str">
+      <c r="BI2" t="str">
         <v>most recent travel return date</v>
       </c>
-      <c r="BI2" t="str">
+      <c r="BJ2" t="str">
         <v>travel history</v>
       </c>
-      <c r="BJ2" t="str">
+      <c r="BK2" t="str">
         <v>exposure event</v>
       </c>
-      <c r="BK2" t="str">
+      <c r="BL2" t="str">
         <v>direct/indirect exposure</v>
       </c>
-      <c r="BL2" t="str">
+      <c r="BM2" t="str">
         <v>host role</v>
       </c>
-      <c r="BM2" t="str">
+      <c r="BN2" t="str">
         <v>exposure setting</v>
       </c>
-      <c r="BN2" t="str">
+      <c r="BO2" t="str">
         <v>exposure details</v>
       </c>
-      <c r="BO2" t="str">
+      <c r="BP2" t="str">
         <v>purpose of sequencing</v>
       </c>
-      <c r="BP2" t="str">
+      <c r="BQ2" t="str">
         <v>library ID</v>
       </c>
-      <c r="BQ2" t="str">
+      <c r="BR2" t="str">
         <v>library insert size</v>
       </c>
-      <c r="BR2" t="str">
+      <c r="BS2" t="str">
         <v>library preparation method</v>
       </c>
-      <c r="BS2" t="str">
+      <c r="BT2" t="str">
         <v>MinIon barcode</v>
       </c>
-      <c r="BT2" t="str">
+      <c r="BU2" t="str">
         <v>sequencing instrument</v>
       </c>
-      <c r="BU2" t="str">
+      <c r="BV2" t="str">
         <v>sequencing protocol name</v>
       </c>
-      <c r="BV2" t="str">
+      <c r="BW2" t="str">
         <v>sequencing protocol source</v>
       </c>
-      <c r="BW2" t="str">
+      <c r="BX2" t="str">
         <v>sequencing kit number</v>
       </c>
-      <c r="BX2" t="str">
+      <c r="BY2" t="str">
         <v>amplicon pcr primers filename</v>
       </c>
-      <c r="BY2" t="str">
+      <c r="BZ2" t="str">
         <v>sample sequenced date</v>
       </c>
-      <c r="BZ2" t="str">
+      <c r="CA2" t="str">
         <v>raw sequence data processing</v>
       </c>
-      <c r="CA2" t="str">
+      <c r="CB2" t="str">
         <v>sequencing depth (average)</v>
       </c>
-      <c r="CB2" t="str">
+      <c r="CC2" t="str">
         <v>assembly name</v>
       </c>
-      <c r="CC2" t="str">
+      <c r="CD2" t="str">
         <v>assembly method</v>
       </c>
-      <c r="CD2" t="str">
+      <c r="CE2" t="str">
         <v>assembly coverage breadth</v>
       </c>
-      <c r="CE2" t="str">
+      <c r="CF2" t="str">
         <v>assembly coverage depth</v>
       </c>
-      <c r="CF2" t="str">
+      <c r="CG2" t="str">
         <v>r1 fastq filename</v>
       </c>
-      <c r="CG2" t="str">
+      <c r="CH2" t="str">
         <v>r2 fastq filename</v>
       </c>
-      <c r="CH2" t="str">
+      <c r="CI2" t="str">
         <v>r1 fastq filepath</v>
       </c>
-      <c r="CI2" t="str">
+      <c r="CJ2" t="str">
         <v>r2 fastq filepath</v>
       </c>
-      <c r="CJ2" t="str">
+      <c r="CK2" t="str">
         <v>fast5 filename</v>
       </c>
-      <c r="CK2" t="str">
+      <c r="CL2" t="str">
         <v>fast5 filepath</v>
       </c>
-      <c r="CL2" t="str">
+      <c r="CM2" t="str">
         <v>fasta filename</v>
       </c>
-      <c r="CM2" t="str">
+      <c r="CN2" t="str">
         <v>fasta filepath</v>
       </c>
-      <c r="CN2" t="str">
+      <c r="CO2" t="str">
         <v>number base pairs</v>
       </c>
-      <c r="CO2" t="str">
+      <c r="CP2" t="str">
         <v>consensus genome length</v>
       </c>
-      <c r="CP2" t="str">
+      <c r="CQ2" t="str">
         <v>mean contig length</v>
       </c>
-      <c r="CQ2" t="str">
+      <c r="CR2" t="str">
         <v>N50</v>
       </c>
-      <c r="CR2" t="str">
+      <c r="CS2" t="str">
         <v>Ns per 100 kbp</v>
       </c>
-      <c r="CS2" t="str">
+      <c r="CT2" t="str">
         <v>reference genome accession</v>
       </c>
-      <c r="CT2" t="str">
+      <c r="CU2" t="str">
         <v>consensus sequence ID</v>
       </c>
-      <c r="CU2" t="str">
+      <c r="CV2" t="str">
         <v>consensus sequence method</v>
       </c>
-      <c r="CV2" t="str">
+      <c r="CW2" t="str">
         <v>consensus sequence filename</v>
       </c>
-      <c r="CW2" t="str">
+      <c r="CX2" t="str">
         <v>consensus sequence filepath</v>
       </c>
-      <c r="CX2" t="str">
+      <c r="CY2" t="str">
         <v>annotation feature table filename</v>
       </c>
-      <c r="CY2" t="str">
+      <c r="CZ2" t="str">
         <v>bioinformatics protocol</v>
       </c>
-      <c r="CZ2" t="str">
+      <c r="DA2" t="str">
         <v>gene name 1</v>
       </c>
-      <c r="DA2" t="str">
+      <c r="DB2" t="str">
         <v>diagnostic pcr protocol 1</v>
       </c>
-      <c r="DB2" t="str">
+      <c r="DC2" t="str">
         <v>diagnostic pcr Ct value 1</v>
       </c>
-      <c r="DC2" t="str">
+      <c r="DD2" t="str">
         <v>gene name 2</v>
       </c>
-      <c r="DD2" t="str">
+      <c r="DE2" t="str">
         <v>diagnostic pcr protocol 2</v>
       </c>
-      <c r="DE2" t="str">
+      <c r="DF2" t="str">
         <v>diagnostic pcr Ct value 2</v>
       </c>
-      <c r="DF2" t="str">
+      <c r="DG2" t="str">
         <v>authors</v>
       </c>
-      <c r="DG2" t="str">
+      <c r="DH2" t="str">
         <v>DataHarmonizer provenance</v>
       </c>
     </row>
@@ -1190,198 +1196,201 @@
         <v>76</v>
       </c>
       <c r="AU3" t="str">
+        <v/>
+      </c>
+      <c r="AV3" t="str">
         <v>70 - 79</v>
       </c>
-      <c r="AV3" t="str">
+      <c r="AW3" t="str">
         <v>Female</v>
       </c>
-      <c r="AW3" t="str">
+      <c r="AX3" t="str">
         <v>United States of America</v>
       </c>
-      <c r="AX3" t="str">
+      <c r="AY3" t="str">
         <v>nSQu_4</v>
       </c>
-      <c r="AY3" t="str">
+      <c r="AZ3" t="str">
         <v>2020-03-05</v>
       </c>
-      <c r="AZ3" t="str">
+      <c r="BA3" t="str">
         <v>Ageusia (complete loss of taste); Conjunctivitis (pink eye); Cough; Headache; Hypotension (low blood pressure)</v>
       </c>
-      <c r="BA3" t="str">
+      <c r="BB3" t="str">
         <v>Age 60+; Metastatic disease; Smoking</v>
       </c>
-      <c r="BB3" t="str">
+      <c r="BC3" t="str">
         <v>Acute respiratory failure; Guillain-Barré syndrome</v>
       </c>
-      <c r="BC3" t="str">
+      <c r="BD3" t="str">
         <v>United States of America</v>
       </c>
-      <c r="BD3" t="str">
+      <c r="BE3" t="str">
         <v>New York City</v>
       </c>
-      <c r="BE3" t="str">
+      <c r="BF3" t="str">
         <v>State of New York</v>
       </c>
-      <c r="BF3" t="str">
+      <c r="BG3" t="str">
         <v>United States of America</v>
       </c>
-      <c r="BG3" t="str">
+      <c r="BH3" t="str">
         <v>2020-07-14</v>
       </c>
-      <c r="BH3" t="str">
+      <c r="BI3" t="str">
         <v>2020-07-23</v>
       </c>
-      <c r="BI3" t="str">
+      <c r="BJ3" t="str">
         <v>Canada, Yellowknife; Canada, Fort Providence: USA, Bismarck</v>
       </c>
-      <c r="BJ3" t="str">
+      <c r="BK3" t="str">
         <v>Missing</v>
       </c>
-      <c r="BK3" t="str">
+      <c r="BL3" t="str">
         <v>Indirect</v>
       </c>
-      <c r="BL3" t="str">
+      <c r="BM3" t="str">
         <v>Patient</v>
       </c>
-      <c r="BM3" t="str">
+      <c r="BN3" t="str">
         <v>Patient Contact</v>
       </c>
-      <c r="BN3" t="str">
+      <c r="BO3" t="str">
         <v>Exposure setting - in the same common room.</v>
       </c>
-      <c r="BO3" t="str">
+      <c r="BP3" t="str">
         <v>Cluster investigation</v>
       </c>
-      <c r="BP3" t="str">
+      <c r="BQ3" t="str">
         <v>Timor-Leste-Handrail-860-1</v>
       </c>
-      <c r="BQ3" t="str">
+      <c r="BR3" t="str">
         <v>300</v>
       </c>
-      <c r="BR3" t="str">
+      <c r="BS3" t="str">
         <v>Nextera XT</v>
       </c>
-      <c r="BS3" t="str">
+      <c r="BT3" t="str">
         <v>3225848155</v>
       </c>
-      <c r="BT3" t="str">
+      <c r="BU3" t="str">
         <v>DNBSEQ-G50</v>
       </c>
-      <c r="BU3" t="str">
+      <c r="BV3" t="str">
         <v>NGS protocol v. 12</v>
       </c>
-      <c r="BV3" t="str">
+      <c r="BW3" t="str">
         <v>NGS Libraries</v>
       </c>
-      <c r="BW3" t="str">
+      <c r="BX3" t="str">
         <v>NG5T1LK633</v>
       </c>
-      <c r="BX3" t="str">
+      <c r="BY3" t="str">
         <v>Timor-Leste860_2020-02.txt</v>
       </c>
-      <c r="BY3" t="str">
+      <c r="BZ3" t="str">
         <v>2020-09-01</v>
       </c>
-      <c r="BZ3" t="str">
+      <c r="CA3" t="str">
         <v>Porechop v. 0.2.3</v>
       </c>
-      <c r="CA3" t="str">
+      <c r="CB3" t="str">
         <v>99x</v>
       </c>
-      <c r="CB3" t="str">
+      <c r="CC3" t="str">
         <v>timor-leste-handrail-86039assembly.fasta</v>
       </c>
-      <c r="CC3" t="str">
+      <c r="CD3" t="str">
         <v>Shovil</v>
       </c>
-      <c r="CD3" t="str">
+      <c r="CE3" t="str">
         <v>91%</v>
       </c>
-      <c r="CE3" t="str">
+      <c r="CF3" t="str">
         <v>17x</v>
       </c>
-      <c r="CF3" t="str">
+      <c r="CG3" t="str">
         <v>Timor-Leste860_S1_L001_R1_001.fastq.gz</v>
       </c>
-      <c r="CG3" t="str">
+      <c r="CH3" t="str">
         <v>Timor-Leste860_S1_L001_R2_001.fastq.gz</v>
       </c>
-      <c r="CH3" t="str">
+      <c r="CI3" t="str">
         <v>/Users/Matthew James/Documents/I./stay dark.fastq.gz</v>
       </c>
-      <c r="CI3" t="str">
+      <c r="CJ3" t="str">
         <v>/Users/Heather Gonzalez/Downloads/Development$/</v>
       </c>
-      <c r="CJ3" t="str">
+      <c r="CK3" t="str">
         <v>Timor-Leste860_2020-02_batch1a.fast5</v>
       </c>
-      <c r="CK3" t="str">
+      <c r="CL3" t="str">
         <v>/Users/Snyder/Downloads/Concern/.fast5</v>
       </c>
-      <c r="CL3" t="str">
+      <c r="CM3" t="str">
         <v>Timor-Leste860_2020-02_batch1a.fasta</v>
       </c>
-      <c r="CM3" t="str">
+      <c r="CN3" t="str">
         <v>/Users/Phillip Barry/Desktop/</v>
       </c>
-      <c r="CN3" t="str">
+      <c r="CO3" t="str">
         <v>185272</v>
       </c>
-      <c r="CO3" t="str">
+      <c r="CP3" t="str">
         <v>2566</v>
       </c>
-      <c r="CP3" t="str">
+      <c r="CQ3" t="str">
         <v>21180</v>
       </c>
-      <c r="CQ3" t="str">
+      <c r="CR3" t="str">
         <v>601</v>
       </c>
-      <c r="CR3" t="str">
+      <c r="CS3" t="str">
         <v>865.61</v>
       </c>
-      <c r="CS3" t="str">
+      <c r="CT3" t="str">
         <v>MT_419846.1</v>
       </c>
-      <c r="CT3" t="str">
+      <c r="CU3" t="str">
         <v>SARS-CoV-2_MT3989</v>
       </c>
-      <c r="CU3" t="str">
+      <c r="CV3" t="str">
         <v>CASAVA v. 1.8.2</v>
       </c>
-      <c r="CV3" t="str">
+      <c r="CW3" t="str">
         <v>SARS-CoV-2_MT3989.fasta</v>
       </c>
-      <c r="CW3" t="str">
+      <c r="CX3" t="str">
         <v>/Users/Jacqueline/Desktop/Work/Seq/Consensus/</v>
       </c>
-      <c r="CX3" t="str">
+      <c r="CY3" t="str">
         <v>Timor-Leste860_2020-02_Annotation-Features.tbl</v>
       </c>
-      <c r="CY3" t="str">
+      <c r="CZ3" t="str">
         <v>Whole-exome-sequencing-and-bioinformatics-analysis-jhscj6e</v>
       </c>
-      <c r="CZ3" t="str">
+      <c r="DA3" t="str">
         <v>nsp12 (RdRp)</v>
       </c>
-      <c r="DA3" t="str">
+      <c r="DB3" t="str">
         <v>Severe acute respiratory syndrome coronavirus 2 (SARS-CoV-2) RdRp nested RT-PCR V.2</v>
       </c>
-      <c r="DB3" t="str">
+      <c r="DC3" t="str">
         <v>13</v>
       </c>
-      <c r="DC3" t="str">
+      <c r="DD3" t="str">
         <v>ORF7b (ns7b)</v>
       </c>
-      <c r="DD3" t="str">
+      <c r="DE3" t="str">
         <v>SARS-CoV-2 RT-PCR ORF7b 2020 (Wuhan-ORF1ab; 2019-nCoV-related test version 0.3.0</v>
       </c>
-      <c r="DE3" t="str">
+      <c r="DF3" t="str">
         <v>6</v>
       </c>
-      <c r="DF3" t="str">
+      <c r="DG3" t="str">
         <v>Diana Tucker, Ashley McIntyre, Sandra Smith, Christopher Brown, Robert North, Christopher Green</v>
       </c>
-      <c r="DG3" t="str">
+      <c r="DH3" t="str">
         <v>DataHarmonizer: v0.13.3</v>
       </c>
     </row>
@@ -1525,198 +1534,201 @@
         <v>89</v>
       </c>
       <c r="AU4" t="str">
+        <v/>
+      </c>
+      <c r="AV4" t="str">
         <v>80 - 89</v>
       </c>
-      <c r="AV4" t="str">
+      <c r="AW4" t="str">
         <v>Non-binary gender</v>
       </c>
-      <c r="AW4" t="str">
+      <c r="AX4" t="str">
         <v>Bosnia and Herzegovina</v>
       </c>
-      <c r="AX4" t="str">
+      <c r="AY4" t="str">
         <v>rblyp6</v>
       </c>
-      <c r="AY4" t="str">
+      <c r="AZ4" t="str">
         <v>2020-03-08</v>
       </c>
-      <c r="AZ4" t="str">
+      <c r="BA4" t="str">
         <v>Confusion; Chills (sudden cold sensation); Cough; Arthralgia (painful joints); Myalgia (muscle pain); Pharyngitis (sore throat)</v>
       </c>
-      <c r="BA4" t="str">
+      <c r="BB4" t="str">
         <v>Bone marrow failure; Metastatic disease; Cardiac disease</v>
       </c>
-      <c r="BB4" t="str">
+      <c r="BC4" t="str">
         <v>Kawasaki disease</v>
       </c>
-      <c r="BC4" t="str">
+      <c r="BD4" t="str">
         <v>Japan</v>
       </c>
-      <c r="BD4" t="str">
+      <c r="BE4" t="str">
         <v>Montreal</v>
       </c>
-      <c r="BE4" t="str">
+      <c r="BF4" t="str">
         <v>Quebec</v>
       </c>
-      <c r="BF4" t="str">
+      <c r="BG4" t="str">
         <v>Canada</v>
       </c>
-      <c r="BG4" t="str">
+      <c r="BH4" t="str">
         <v>2020-05-24</v>
       </c>
-      <c r="BH4" t="str">
+      <c r="BI4" t="str">
         <v>2020-05-02</v>
       </c>
-      <c r="BI4" t="str">
+      <c r="BJ4" t="str">
         <v>Canada, Alberta; Japan, Tokyo</v>
       </c>
-      <c r="BJ4" t="str">
+      <c r="BK4" t="str">
         <v>Community Event</v>
       </c>
-      <c r="BK4" t="str">
+      <c r="BL4" t="str">
         <v>Direct</v>
       </c>
-      <c r="BL4" t="str">
+      <c r="BM4" t="str">
         <v>Other</v>
       </c>
-      <c r="BM4" t="str">
+      <c r="BN4" t="str">
         <v>First Nations Reserve</v>
       </c>
-      <c r="BN4" t="str">
+      <c r="BO4" t="str">
         <v>Host role - Other: Gardener</v>
       </c>
-      <c r="BO4" t="str">
+      <c r="BP4" t="str">
         <v>Diagnostic testing</v>
       </c>
-      <c r="BP4" t="str">
+      <c r="BQ4" t="str">
         <v>NewBrunswick-Severeacuterespiratoryvirus2-416;3</v>
       </c>
-      <c r="BQ4" t="str">
+      <c r="BR4" t="str">
         <v>200</v>
       </c>
-      <c r="BR4" t="str">
+      <c r="BS4" t="str">
         <v>NEBNext Ultra II</v>
       </c>
-      <c r="BS4" t="str">
+      <c r="BT4" t="str">
         <v>5199601997</v>
       </c>
-      <c r="BT4" t="str">
+      <c r="BU4" t="str">
         <v>HiSeq X Ten</v>
       </c>
-      <c r="BU4" t="str">
+      <c r="BV4" t="str">
         <v>Seq System Protocol v. 0.1.4</v>
       </c>
-      <c r="BV4" t="str">
+      <c r="BW4" t="str">
         <v>BFX-UT_ARTIC_Illumina V 10.4</v>
       </c>
-      <c r="BW4" t="str">
+      <c r="BX4" t="str">
         <v>BDI5MLQMCI6</v>
       </c>
-      <c r="BX4" t="str">
+      <c r="BY4" t="str">
         <v>NB_SARSCoV2-416_2020ampli.txt</v>
       </c>
-      <c r="BY4" t="str">
+      <c r="BZ4" t="str">
         <v>2020-10-20</v>
       </c>
-      <c r="BZ4" t="str">
+      <c r="CA4" t="str">
         <v>Deepbinner v. 0.2.0</v>
       </c>
-      <c r="CA4" t="str">
+      <c r="CB4" t="str">
         <v>19x</v>
       </c>
-      <c r="CB4" t="str">
+      <c r="CC4" t="str">
         <v>newbrunswick-severeacuterespiratoryvirus2-41628assembly.fasta</v>
       </c>
-      <c r="CC4" t="str">
+      <c r="CD4" t="str">
         <v>Canu</v>
       </c>
-      <c r="CD4" t="str">
+      <c r="CE4" t="str">
         <v>20%</v>
       </c>
-      <c r="CE4" t="str">
+      <c r="CF4" t="str">
         <v>15x</v>
       </c>
-      <c r="CF4" t="str">
+      <c r="CG4" t="str">
         <v>NB_SARSCoV2-416_S2_L020_R1_001.fasta.gz</v>
       </c>
-      <c r="CG4" t="str">
+      <c r="CH4" t="str">
         <v>NB_SARSCoV2-416_S2_L020_R2_001.fasta.gz</v>
       </c>
-      <c r="CH4" t="str">
+      <c r="CI4" t="str">
         <v>/Users/Robert/Downloads/unit-/where item.fastq.gz</v>
       </c>
-      <c r="CI4" t="str">
+      <c r="CJ4" t="str">
         <v>/Users/Baker/Desktop/"/town-small-consider-wife.fastq.gz</v>
       </c>
-      <c r="CJ4" t="str">
+      <c r="CK4" t="str">
         <v>NB_SARSCoV2-416_2020-seq.fast5</v>
       </c>
-      <c r="CK4" t="str">
+      <c r="CL4" t="str">
         <v>/Users/Kim/Google Drive/his/local-method.fast5</v>
       </c>
-      <c r="CL4" t="str">
+      <c r="CM4" t="str">
         <v>NB_SARSCoV2-416_2020-seq.fasta</v>
       </c>
-      <c r="CM4" t="str">
+      <c r="CN4" t="str">
         <v>/Users/Stephanie/Downloads/NB_SARSCoV2-416_2020-seq.fasta</v>
       </c>
-      <c r="CN4" t="str">
+      <c r="CO4" t="str">
         <v>219669</v>
       </c>
-      <c r="CO4" t="str">
+      <c r="CP4" t="str">
         <v>3787</v>
       </c>
-      <c r="CP4" t="str">
+      <c r="CQ4" t="str">
         <v>12664</v>
       </c>
-      <c r="CQ4" t="str">
+      <c r="CR4" t="str">
         <v>1214</v>
       </c>
-      <c r="CR4" t="str">
+      <c r="CS4" t="str">
         <v>831.4</v>
       </c>
-      <c r="CS4" t="str">
+      <c r="CT4" t="str">
         <v>NC_045512.1</v>
       </c>
-      <c r="CT4" t="str">
+      <c r="CU4" t="str">
         <v>ConsensusSeq_U0K724</v>
       </c>
-      <c r="CU4" t="str">
+      <c r="CV4" t="str">
         <v>Carthagene v. 1.2</v>
       </c>
-      <c r="CV4" t="str">
+      <c r="CW4" t="str">
         <v>ConsensusSeq_U0K724.fasta</v>
       </c>
-      <c r="CW4" t="str">
+      <c r="CX4" t="str">
         <v>/Users/Haley/Google Drive/ConsensusSeq_U0K724.fasta</v>
       </c>
-      <c r="CX4" t="str">
+      <c r="CY4" t="str">
         <v>NB_SARSCoV2-416_2020-seq-AFT.tbl</v>
       </c>
-      <c r="CY4" t="str">
+      <c r="CZ4" t="str">
         <v>Assessing sequence quality in galaxytrakr v 1.2</v>
       </c>
-      <c r="CZ4" t="str">
+      <c r="DA4" t="str">
         <v>ORF7a</v>
       </c>
-      <c r="DA4" t="str">
+      <c r="DB4" t="str">
         <v>AllTheTestingPCRing-orf7a v. 2</v>
       </c>
-      <c r="DB4" t="str">
+      <c r="DC4" t="str">
         <v>37</v>
       </c>
-      <c r="DC4" t="str">
+      <c r="DD4" t="str">
         <v>Spike (orf2)</v>
       </c>
-      <c r="DD4" t="str">
+      <c r="DE4" t="str">
         <v>2019-nCoV ORF2-gene-v.10</v>
       </c>
-      <c r="DE4" t="str">
+      <c r="DF4" t="str">
         <v>36</v>
       </c>
-      <c r="DF4" t="str">
+      <c r="DG4" t="str">
         <v>Clyde D. Flores, Tami L. Logan, Amelia M. Foster</v>
       </c>
-      <c r="DG4" t="str">
+      <c r="DH4" t="str">
         <v>DataHarmonizer: v0.13.3</v>
       </c>
     </row>
@@ -1860,198 +1872,201 @@
         <v>61</v>
       </c>
       <c r="AU5" t="str">
+        <v/>
+      </c>
+      <c r="AV5" t="str">
         <v>60 - 69</v>
       </c>
-      <c r="AV5" t="str">
+      <c r="AW5" t="str">
         <v>Undeclared</v>
       </c>
-      <c r="AW5" t="str">
+      <c r="AX5" t="str">
         <v>Kingman Reef</v>
       </c>
-      <c r="AX5" t="str">
+      <c r="AY5" t="str">
         <v>GeV:6</v>
       </c>
-      <c r="AY5" t="str">
+      <c r="AZ5" t="str">
         <v>2020-01-10</v>
       </c>
-      <c r="AZ5" t="str">
+      <c r="BA5" t="str">
         <v>Dyspnea (breathing difficulty); Malaise (general discomfort/unease); Rhinorrhea (runny nose); Tachypnea (accelerated respiratory rate); Vomiting (throwing up)</v>
       </c>
-      <c r="BA5" t="str">
+      <c r="BB5" t="str">
         <v>Anemia</v>
       </c>
-      <c r="BB5" t="str">
+      <c r="BC5" t="str">
         <v>Abnormal blood oxygen level</v>
       </c>
-      <c r="BC5" t="str">
+      <c r="BD5" t="str">
         <v>Canada</v>
       </c>
-      <c r="BD5" t="str">
+      <c r="BE5" t="str">
         <v>Dublin</v>
       </c>
-      <c r="BE5" t="str">
+      <c r="BF5" t="str">
         <v>Dublin Region</v>
       </c>
-      <c r="BF5" t="str">
+      <c r="BG5" t="str">
         <v>Ireland</v>
       </c>
-      <c r="BG5" t="str">
+      <c r="BH5" t="str">
         <v>2020-10-15</v>
       </c>
-      <c r="BH5" t="str">
+      <c r="BI5" t="str">
         <v>2020-10-30</v>
       </c>
-      <c r="BI5" t="str">
+      <c r="BJ5" t="str">
         <v>Canada, New Brunswick</v>
       </c>
-      <c r="BJ5" t="str">
+      <c r="BK5" t="str">
         <v>Other</v>
       </c>
-      <c r="BK5" t="str">
+      <c r="BL5" t="str">
         <v>Direct</v>
       </c>
-      <c r="BL5" t="str">
+      <c r="BM5" t="str">
         <v>Administrator</v>
       </c>
-      <c r="BM5" t="str">
+      <c r="BN5" t="str">
         <v>Daycare</v>
       </c>
-      <c r="BN5" t="str">
+      <c r="BO5" t="str">
         <v>Direct contact with COVID-19 positive visitor at place of wokr.</v>
       </c>
-      <c r="BO5" t="str">
+      <c r="BP5" t="str">
         <v>Research</v>
       </c>
-      <c r="BP5" t="str">
+      <c r="BQ5" t="str">
         <v>ABC-6543211</v>
       </c>
-      <c r="BQ5" t="str">
+      <c r="BR5" t="str">
         <v>260</v>
       </c>
-      <c r="BR5" t="str">
+      <c r="BS5" t="str">
         <v>NEBNext Ultra I</v>
       </c>
-      <c r="BS5" t="str">
+      <c r="BT5" t="str">
         <v>6476849764</v>
       </c>
-      <c r="BT5" t="str">
+      <c r="BU5" t="str">
         <v>Illumina Genome Analyzer II</v>
       </c>
-      <c r="BU5" t="str">
+      <c r="BV5" t="str">
         <v>Super Duper Prot. v.1.9</v>
       </c>
-      <c r="BV5" t="str">
+      <c r="BW5" t="str">
         <v>ARTIC Network</v>
       </c>
-      <c r="BW5" t="str">
+      <c r="BX5" t="str">
         <v>CO32934396</v>
       </c>
-      <c r="BX5" t="str">
+      <c r="BY5" t="str">
         <v>Mali_RmYN02_eaqr-amplicon.txt</v>
       </c>
-      <c r="BY5" t="str">
+      <c r="BZ5" t="str">
         <v>2020-08-31</v>
       </c>
-      <c r="BZ5" t="str">
+      <c r="CA5" t="str">
         <v>Guppy v. 0.5.1</v>
       </c>
-      <c r="CA5" t="str">
+      <c r="CB5" t="str">
         <v>116x</v>
       </c>
-      <c r="CB5" t="str">
+      <c r="CC5" t="str">
         <v>mali_rmyn02_eaqr1assembly.fasta</v>
       </c>
-      <c r="CC5" t="str">
+      <c r="CD5" t="str">
         <v>Velvet</v>
       </c>
-      <c r="CD5" t="str">
+      <c r="CE5" t="str">
         <v>83.65%</v>
       </c>
-      <c r="CE5" t="str">
+      <c r="CF5" t="str">
         <v>111x</v>
       </c>
-      <c r="CF5" t="str">
+      <c r="CG5" t="str">
         <v>Mali-RmYN02eaqr_S1_L001_R1_001.fastq.gz</v>
       </c>
-      <c r="CG5" t="str">
+      <c r="CH5" t="str">
         <v>Mali-RmYN02eaqr_S1_L001_R2_001.fastq.gz</v>
       </c>
-      <c r="CH5" t="str">
+      <c r="CI5" t="str">
         <v>/Users/Lori/Documents/</v>
       </c>
-      <c r="CI5" t="str">
+      <c r="CJ5" t="str">
         <v>/Users/Monica Kelley/Google Drive/staff/girl.fastq.gz</v>
       </c>
-      <c r="CJ5" t="str">
+      <c r="CK5" t="str">
         <v>Mali_RmYN02_eaqr-batch2b.fast5</v>
       </c>
-      <c r="CK5" t="str">
+      <c r="CL5" t="str">
         <v>/Users/Hurley/Downloads/seq/</v>
       </c>
-      <c r="CL5" t="str">
+      <c r="CM5" t="str">
         <v>Mali_RmYN02_eaqr-batch2b.fasta</v>
       </c>
-      <c r="CM5" t="str">
+      <c r="CN5" t="str">
         <v>/Users/James/Downloads/be/</v>
       </c>
-      <c r="CN5" t="str">
+      <c r="CO5" t="str">
         <v>157621</v>
       </c>
-      <c r="CO5" t="str">
+      <c r="CP5" t="str">
         <v>6672</v>
       </c>
-      <c r="CP5" t="str">
+      <c r="CQ5" t="str">
         <v>5799</v>
       </c>
-      <c r="CQ5" t="str">
+      <c r="CR5" t="str">
         <v>1887</v>
       </c>
-      <c r="CR5" t="str">
+      <c r="CS5" t="str">
         <v>419.92</v>
       </c>
-      <c r="CS5" t="str">
+      <c r="CT5" t="str">
         <v>MN988668</v>
       </c>
-      <c r="CT5" t="str">
+      <c r="CU5" t="str">
         <v>SARS-CoV-2_GWA665</v>
       </c>
-      <c r="CU5" t="str">
+      <c r="CV5" t="str">
         <v>FALCON v0.1</v>
       </c>
-      <c r="CV5" t="str">
+      <c r="CW5" t="str">
         <v>SARS-CoV-2_GWA665.fasta</v>
       </c>
-      <c r="CW5" t="str">
+      <c r="CX5" t="str">
         <v>/Users/Watts/Documents/DEN/</v>
       </c>
-      <c r="CX5" t="str">
+      <c r="CY5" t="str">
         <v>Mali_RmYN02_eaqr-annotation.tbl</v>
       </c>
-      <c r="CY5" t="str">
+      <c r="CZ5" t="str">
         <v>Pacbio long-read sequencing 0.2.6</v>
       </c>
-      <c r="CZ5" t="str">
+      <c r="DA5" t="str">
         <v>N (orf9)</v>
       </c>
-      <c r="DA5" t="str">
+      <c r="DB5" t="str">
         <v>SARS-CoV-2 real-time RT-PCR N gene 2020 (2019-nCoV-related test) V.2</v>
       </c>
-      <c r="DB5" t="str">
+      <c r="DC5" t="str">
         <v>28</v>
       </c>
-      <c r="DC5" t="str">
+      <c r="DD5" t="str">
         <v>ORF6 (ns6)</v>
       </c>
-      <c r="DD5" t="str">
+      <c r="DE5" t="str">
         <v>Withalwaysnote_V 6</v>
       </c>
-      <c r="DE5" t="str">
+      <c r="DF5" t="str">
         <v>6</v>
       </c>
-      <c r="DF5" t="str">
+      <c r="DG5" t="str">
         <v>Margaret Holder</v>
       </c>
-      <c r="DG5" t="str">
+      <c r="DH5" t="str">
         <v>DataHarmonizer: v0.13.3</v>
       </c>
     </row>
@@ -2195,198 +2210,201 @@
         <v>84</v>
       </c>
       <c r="AU6" t="str">
+        <v/>
+      </c>
+      <c r="AV6" t="str">
         <v>80 - 89</v>
       </c>
-      <c r="AV6" t="str">
+      <c r="AW6" t="str">
         <v>Male</v>
       </c>
-      <c r="AW6" t="str">
+      <c r="AX6" t="str">
         <v>Canada</v>
       </c>
-      <c r="AX6" t="str">
+      <c r="AY6" t="str">
         <v>007-Gld-6</v>
       </c>
-      <c r="AY6" t="str">
+      <c r="AZ6" t="str">
         <v>2020-02-22</v>
       </c>
-      <c r="AZ6" t="str">
+      <c r="BA6" t="str">
         <v>Confusion; Irritability; Asthenia (general weakness); Cough</v>
       </c>
-      <c r="BA6" t="str">
+      <c r="BB6" t="str">
         <v>Hypertension (high blood pressure); Postpartum (≤6 weeks)</v>
       </c>
-      <c r="BB6" t="str">
+      <c r="BC6" t="str">
         <v>COVID-19 associated ARDS (CARDS); Cardiac injury; Cardiac arrest</v>
       </c>
-      <c r="BC6" t="str">
+      <c r="BD6" t="str">
         <v>Kosovo</v>
       </c>
-      <c r="BD6" t="str">
+      <c r="BE6" t="str">
         <v>Nice</v>
       </c>
-      <c r="BE6" t="str">
+      <c r="BF6" t="str">
         <v>Provence-Alpes-Cote d'Azur Region</v>
       </c>
-      <c r="BF6" t="str">
+      <c r="BG6" t="str">
         <v>France</v>
       </c>
-      <c r="BG6" t="str">
+      <c r="BH6" t="str">
         <v>2020-09-01</v>
       </c>
-      <c r="BH6" t="str">
+      <c r="BI6" t="str">
         <v>2020-09-03</v>
       </c>
-      <c r="BI6" t="str">
+      <c r="BJ6" t="str">
         <v>Canada, Herchmer; Canada, Montreal; Kosovo, Prishtina</v>
       </c>
-      <c r="BJ6" t="str">
+      <c r="BK6" t="str">
         <v>Not Applicable</v>
       </c>
-      <c r="BK6" t="str">
+      <c r="BL6" t="str">
         <v>Unknown</v>
       </c>
-      <c r="BL6" t="str">
+      <c r="BM6" t="str">
         <v>First Responder</v>
       </c>
-      <c r="BM6" t="str">
+      <c r="BN6" t="str">
         <v>Household</v>
       </c>
-      <c r="BN6" t="str">
+      <c r="BO6" t="str">
         <v>Exposure setting - visited personal home for work duty.</v>
       </c>
-      <c r="BO6" t="str">
+      <c r="BP6" t="str">
         <v>Surveillance testing</v>
       </c>
-      <c r="BP6" t="str">
+      <c r="BQ6" t="str">
         <v>Newfoundland_Bronchoscope_IskH_007</v>
       </c>
-      <c r="BQ6" t="str">
+      <c r="BR6" t="str">
         <v>187</v>
       </c>
-      <c r="BR6" t="str">
+      <c r="BS6" t="str">
         <v>Collibri PS DNA Library Prep Kit</v>
       </c>
-      <c r="BS6" t="str">
+      <c r="BT6" t="str">
         <v>3821789592</v>
       </c>
-      <c r="BT6" t="str">
+      <c r="BU6" t="str">
         <v>Ion Torrent S5 XL</v>
       </c>
-      <c r="BU6" t="str">
+      <c r="BV6" t="str">
         <v>pro-seq tech protocol v. 8</v>
       </c>
-      <c r="BV6" t="str">
+      <c r="BW6" t="str">
         <v>NGS protocol v.5.0</v>
       </c>
-      <c r="BW6" t="str">
+      <c r="BX6" t="str">
         <v>LS-2CUO1B</v>
       </c>
-      <c r="BX6" t="str">
+      <c r="BY6" t="str">
         <v>Newfoundland_B-IskH_primer_2020-03.txt</v>
       </c>
-      <c r="BY6" t="str">
+      <c r="BZ6" t="str">
         <v>2020-10-15</v>
       </c>
-      <c r="BZ6" t="str">
+      <c r="CA6" t="str">
         <v>Cutadapt v. 2.10</v>
       </c>
-      <c r="CA6" t="str">
+      <c r="CB6" t="str">
         <v>127x</v>
       </c>
-      <c r="CB6" t="str">
+      <c r="CC6" t="str">
         <v>newfoundland_B-IskH_assembly.fasta</v>
       </c>
-      <c r="CC6" t="str">
+      <c r="CD6" t="str">
         <v>Canu</v>
       </c>
-      <c r="CD6" t="str">
+      <c r="CE6" t="str">
         <v>56.4%</v>
       </c>
-      <c r="CE6" t="str">
+      <c r="CF6" t="str">
         <v>62x</v>
       </c>
-      <c r="CF6" t="str">
+      <c r="CG6" t="str">
         <v>Newfoundland_B-IskH_S1_L103_R1_001.fastq.gz</v>
       </c>
-      <c r="CG6" t="str">
+      <c r="CH6" t="str">
         <v>Newfoundland_B-IskH_S1_L103_R2_001.fastq.gz</v>
       </c>
-      <c r="CH6" t="str">
+      <c r="CI6" t="str">
         <v>/Users/Nathan Lloyd/Documents/</v>
       </c>
-      <c r="CI6" t="str">
+      <c r="CJ6" t="str">
         <v>/Users/Ricky/Google Drive/Window/</v>
       </c>
-      <c r="CJ6" t="str">
+      <c r="CK6" t="str">
         <v>Newfoundland_batch03_B-IskH_2020-03.fast5</v>
       </c>
-      <c r="CK6" t="str">
+      <c r="CL6" t="str">
         <v>/Users/Douglas/Google Drive/test/Newfoundland_batch03_B-IskH_2020-03.fast5</v>
       </c>
-      <c r="CL6" t="str">
+      <c r="CM6" t="str">
         <v>Newfoundland_batch03_B-IskH_2020-03.fasta</v>
       </c>
-      <c r="CM6" t="str">
+      <c r="CN6" t="str">
         <v>/Users/Sandra English/Desktop/Theory/Newfoundland_batch03_B-IskH_2020-03.fasta</v>
       </c>
-      <c r="CN6" t="str">
+      <c r="CO6" t="str">
         <v>336858</v>
       </c>
-      <c r="CO6" t="str">
+      <c r="CP6" t="str">
         <v>15187</v>
       </c>
-      <c r="CP6" t="str">
+      <c r="CQ6" t="str">
         <v>46431</v>
       </c>
-      <c r="CQ6" t="str">
+      <c r="CR6" t="str">
         <v>4921</v>
       </c>
-      <c r="CR6" t="str">
+      <c r="CS6" t="str">
         <v>932.78</v>
       </c>
-      <c r="CS6" t="str">
+      <c r="CT6" t="str">
         <v>SRR80285415</v>
       </c>
-      <c r="CT6" t="str">
+      <c r="CU6" t="str">
         <v>Prov_NOJ678</v>
       </c>
-      <c r="CU6" t="str">
+      <c r="CV6" t="str">
         <v>iVar v. 1.0</v>
       </c>
-      <c r="CV6" t="str">
+      <c r="CW6" t="str">
         <v>Prov_NOJ678-consensus.fasta</v>
       </c>
-      <c r="CW6" t="str">
+      <c r="CX6" t="str">
         <v>/Users/Mclean/Desktop/-/Prov_NOJ678-consensus.fasta</v>
       </c>
-      <c r="CX6" t="str">
+      <c r="CY6" t="str">
         <v>Newfoundland_anno-table_B-IskH_2020-03.tbl</v>
       </c>
-      <c r="CY6" t="str">
+      <c r="CZ6" t="str">
         <v>Ultra-deep-long-read-nanopore-sequencing-of-mock-m-x9tfr6n</v>
       </c>
-      <c r="CZ6" t="str">
+      <c r="DA6" t="str">
         <v>nsp15</v>
       </c>
-      <c r="DA6" t="str">
+      <c r="DB6" t="str">
         <v>2019-nCoV nsp 15 v.10</v>
       </c>
-      <c r="DB6" t="str">
+      <c r="DC6" t="str">
         <v>31</v>
       </c>
-      <c r="DC6" t="str">
+      <c r="DD6" t="str">
         <v>ORF1ab (rep)</v>
       </c>
-      <c r="DD6" t="str">
+      <c r="DE6" t="str">
         <v>SARS-CoV-2 RT-PCR ORF1ab 2020 (Wuhan-ORF1ab; 2019-nCoV-related test V.3</v>
       </c>
-      <c r="DE6" t="str">
+      <c r="DF6" t="str">
         <v>3</v>
       </c>
-      <c r="DF6" t="str">
+      <c r="DG6" t="str">
         <v>Caleb S. Ribush, Abbie Stanley, Gaston Lafond, Cai Shao, Doreen Wexler, Bonanova Aparicio</v>
       </c>
-      <c r="DG6" t="str">
+      <c r="DH6" t="str">
         <v>DataHarmonizer: v0.13.3</v>
       </c>
     </row>
@@ -2530,201 +2548,204 @@
         <v>86</v>
       </c>
       <c r="AU7" t="str">
+        <v/>
+      </c>
+      <c r="AV7" t="str">
         <v>80 - 89</v>
       </c>
-      <c r="AV7" t="str">
+      <c r="AW7" t="str">
         <v>Transgender</v>
       </c>
-      <c r="AW7" t="str">
+      <c r="AX7" t="str">
         <v>Saint Helena</v>
       </c>
-      <c r="AX7" t="str">
+      <c r="AY7" t="str">
         <v>eEn6</v>
       </c>
-      <c r="AY7" t="str">
+      <c r="AZ7" t="str">
         <v>2020-02-13</v>
       </c>
-      <c r="AZ7" t="str">
+      <c r="BA7" t="str">
         <v>Parageusia (distorted sense of taste); Nonproductive cough (dry cough); Dyspnea (breathing difficulty); Encephalitis (brain inflammation); Fever (≥38°C)</v>
       </c>
-      <c r="BA7" t="str">
+      <c r="BB7" t="str">
         <v>Lupus; Sickle cell disease</v>
       </c>
-      <c r="BC7" t="str">
+      <c r="BD7" t="str">
         <v>Canada</v>
       </c>
-      <c r="BD7" t="str">
+      <c r="BE7" t="str">
         <v>Johannesberg</v>
       </c>
-      <c r="BE7" t="str">
+      <c r="BF7" t="str">
         <v>Gauteng Province</v>
       </c>
-      <c r="BF7" t="str">
+      <c r="BG7" t="str">
         <v>South Africa</v>
       </c>
-      <c r="BG7" t="str">
+      <c r="BH7" t="str">
         <v>2020-08-08</v>
       </c>
-      <c r="BH7" t="str">
+      <c r="BI7" t="str">
         <v>2020-08-31</v>
       </c>
-      <c r="BI7" t="str">
+      <c r="BJ7" t="str">
         <v>Canada, Toronto; USA, New York City</v>
       </c>
-      <c r="BJ7" t="str">
+      <c r="BK7" t="str">
         <v>Convention</v>
       </c>
-      <c r="BK7" t="str">
+      <c r="BL7" t="str">
         <v>Indirect</v>
       </c>
-      <c r="BL7" t="str">
+      <c r="BM7" t="str">
         <v>Visitor</v>
       </c>
-      <c r="BM7" t="str">
+      <c r="BN7" t="str">
         <v>Community Service Centre</v>
       </c>
-      <c r="BN7" t="str">
+      <c r="BO7" t="str">
         <v>Attended convention where multiple people where later diagnosed with COVID-19.</v>
       </c>
-      <c r="BO7" t="str">
+      <c r="BP7" t="str">
         <v>Viral passage experiment</v>
       </c>
-      <c r="BP7" t="str">
+      <c r="BQ7" t="str">
         <v>HospitalMissing555-22</v>
       </c>
-      <c r="BQ7" t="str">
+      <c r="BR7" t="str">
         <v>312</v>
       </c>
-      <c r="BR7" t="str">
+      <c r="BS7" t="str">
         <v>QIAseq FX DNA</v>
       </c>
-      <c r="BS7" t="str">
+      <c r="BT7" t="str">
         <v>8439507566</v>
       </c>
-      <c r="BT7" t="str">
+      <c r="BU7" t="str">
         <v>NextSeq 500</v>
       </c>
-      <c r="BU7" t="str">
+      <c r="BV7" t="str">
         <v>ABI xl2500 protocol v. 0.3.5</v>
       </c>
-      <c r="BV7" t="str">
+      <c r="BW7" t="str">
         <v>ABI xl2500 protocol V13</v>
       </c>
-      <c r="BW7" t="str">
+      <c r="BX7" t="str">
         <v>YRPJ-JV6P-HVHT</v>
       </c>
-      <c r="BX7" t="str">
+      <c r="BY7" t="str">
         <v>HospitalMissing555_pcr20.txt</v>
       </c>
-      <c r="BY7" t="str">
+      <c r="BZ7" t="str">
         <v>2020-10-18</v>
       </c>
-      <c r="BZ7" t="str">
+      <c r="CA7" t="str">
         <v>BBTools v. 38.82</v>
       </c>
-      <c r="CA7" t="str">
+      <c r="CB7" t="str">
         <v>129x</v>
       </c>
-      <c r="CB7" t="str">
+      <c r="CC7" t="str">
         <v>hospitalmissing55562assembly.fasta</v>
       </c>
-      <c r="CC7" t="str">
+      <c r="CD7" t="str">
         <v>SPades</v>
       </c>
-      <c r="CD7" t="str">
+      <c r="CE7" t="str">
         <v>32%</v>
       </c>
-      <c r="CE7" t="str">
+      <c r="CF7" t="str">
         <v>4x</v>
       </c>
-      <c r="CF7" t="str">
+      <c r="CG7" t="str">
         <v>HospitalMissing555_S1_L012_R1_001.fastq.gz</v>
       </c>
-      <c r="CG7" t="str">
+      <c r="CH7" t="str">
         <v>HospitalMissing555_S1_L012_R2_001.fastq.gz</v>
       </c>
-      <c r="CH7" t="str">
+      <c r="CI7" t="str">
         <v>/Users/Henry Moss/Desktop/./</v>
       </c>
-      <c r="CI7" t="str">
+      <c r="CJ7" t="str">
         <v>/Users/Brian Cameron/Downloads/form$/light figure degree.fastq.gz</v>
       </c>
-      <c r="CJ7" t="str">
+      <c r="CK7" t="str">
         <v>HospitalMissing555_sequences.fast5</v>
       </c>
-      <c r="CK7" t="str">
+      <c r="CL7" t="str">
         <v>/Users/Walter Bond/Work/</v>
       </c>
-      <c r="CL7" t="str">
+      <c r="CM7" t="str">
         <v>HospitalMissing555_sequences.fasta</v>
       </c>
-      <c r="CM7" t="str">
+      <c r="CN7" t="str">
         <v>/Users/Christopher Martinez/Desktop/administration/</v>
       </c>
-      <c r="CN7" t="str">
+      <c r="CO7" t="str">
         <v>77793</v>
       </c>
-      <c r="CO7" t="str">
+      <c r="CP7" t="str">
         <v>14795</v>
       </c>
-      <c r="CP7" t="str">
+      <c r="CQ7" t="str">
         <v>45791</v>
       </c>
-      <c r="CQ7" t="str">
+      <c r="CR7" t="str">
         <v>4145</v>
       </c>
-      <c r="CR7" t="str">
+      <c r="CS7" t="str">
         <v>652.11</v>
       </c>
-      <c r="CS7" t="str">
+      <c r="CT7" t="str">
         <v>NC_045512.1</v>
       </c>
-      <c r="CT7" t="str">
+      <c r="CU7" t="str">
         <v>ConsensusSeq_EAQ565</v>
       </c>
-      <c r="CU7" t="str">
+      <c r="CV7" t="str">
         <v>CASAVA 1.8.2</v>
       </c>
-      <c r="CV7" t="str">
+      <c r="CW7" t="str">
         <v>ConsensusSeq_EAQ565.fasta</v>
       </c>
-      <c r="CW7" t="str">
+      <c r="CX7" t="str">
         <v>/Users/Dunlap/Downloads/refgenome/</v>
       </c>
-      <c r="CX7" t="str">
+      <c r="CY7" t="str">
         <v>HospitalMissing555_annotations.tbl</v>
       </c>
-      <c r="CY7" t="str">
+      <c r="CZ7" t="str">
         <v>Ncov-2019 sequencing protocol for illumina version 3</v>
       </c>
-      <c r="CZ7" t="str">
+      <c r="DA7" t="str">
         <v>E (orf4)</v>
       </c>
-      <c r="DA7" t="str">
+      <c r="DB7" t="str">
         <v>Severe acute respiratory syndrome coronavirus 2 real-time PCR E gene 2020 v.0.1</v>
       </c>
-      <c r="DB7" t="str">
+      <c r="DC7" t="str">
         <v>4</v>
       </c>
-      <c r="DC7" t="str">
+      <c r="DD7" t="str">
         <v>ORF7a</v>
       </c>
-      <c r="DD7" t="str">
+      <c r="DE7" t="str">
         <v>2019-nCoV orf7a-v. 2</v>
       </c>
-      <c r="DE7" t="str">
+      <c r="DF7" t="str">
         <v>36</v>
       </c>
-      <c r="DF7" t="str">
+      <c r="DG7" t="str">
         <v>Thiery Couture, Xian Ch'iu, G'Kora Zanis</v>
       </c>
-      <c r="DG7" t="str">
+      <c r="DH7" t="str">
         <v>DataHarmonizer: v0.13.3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:DG7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:DH7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated COVID-19 InputData & SOP
- Updated SOP to version 1.5
- Updated COVID-19 inputData files to be compatible with version 0.13.3 and hopefully 0.13.4. Has been modified to uploaded to CNPHI without issues (provided the `DataHarmonizer Provenance` field is manually removed; CNPHI has yet to add this field but it is expected to come soon).
</commit_message>
<xml_diff>
--- a/template/canada_covid19/exampleInput/validTestData.xlsx
+++ b/template/canada_covid19/exampleInput/validTestData.xlsx
@@ -1133,7 +1133,7 @@
         <v>Nucleic acid</v>
       </c>
       <c r="Z3" t="str">
-        <v>Previously Submitted</v>
+        <v>Convalescent</v>
       </c>
       <c r="AA3" t="str">
         <v>Fluid (pleural)</v>
@@ -1193,13 +1193,13 @@
         <v>Missing</v>
       </c>
       <c r="AT3" t="str">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="AU3" t="str">
-        <v/>
+        <v>month</v>
       </c>
       <c r="AV3" t="str">
-        <v>70 - 79</v>
+        <v>0 - 9</v>
       </c>
       <c r="AW3" t="str">
         <v>Female</v>
@@ -1214,7 +1214,7 @@
         <v>2020-03-05</v>
       </c>
       <c r="BA3" t="str">
-        <v>Ageusia (complete loss of taste); Conjunctivitis (pink eye); Cough; Headache; Hypotension (low blood pressure)</v>
+        <v>Ageusia (complete loss of taste); Cough; Headache; Hypotension (low blood pressure)</v>
       </c>
       <c r="BB3" t="str">
         <v>Age 60+; Metastatic disease; Smoking</v>
@@ -1229,7 +1229,7 @@
         <v>New York City</v>
       </c>
       <c r="BF3" t="str">
-        <v>State of New York</v>
+        <v>New York</v>
       </c>
       <c r="BG3" t="str">
         <v>United States of America</v>
@@ -1471,7 +1471,7 @@
         <v>Swab</v>
       </c>
       <c r="Z4" t="str">
-        <v>Previously Submitted</v>
+        <v>Convalescent</v>
       </c>
       <c r="AA4" t="str">
         <v>Missing</v>
@@ -1534,7 +1534,7 @@
         <v>89</v>
       </c>
       <c r="AU4" t="str">
-        <v/>
+        <v>year</v>
       </c>
       <c r="AV4" t="str">
         <v>80 - 89</v>
@@ -1552,7 +1552,7 @@
         <v>2020-03-08</v>
       </c>
       <c r="BA4" t="str">
-        <v>Confusion; Chills (sudden cold sensation); Cough; Arthralgia (painful joints); Myalgia (muscle pain); Pharyngitis (sore throat)</v>
+        <v>Confusion; Cough; Pharyngitis (sore throat)</v>
       </c>
       <c r="BB4" t="str">
         <v>Bone marrow failure; Metastatic disease; Cardiac disease</v>
@@ -1788,10 +1788,10 @@
         <v>2020-05-10</v>
       </c>
       <c r="S5" t="str">
-        <v>Mali</v>
+        <v>Canada</v>
       </c>
       <c r="T5" t="str">
-        <v>Not Applicable</v>
+        <v>Alberta</v>
       </c>
       <c r="U5" t="str">
         <v>Sikasso</v>
@@ -1872,7 +1872,7 @@
         <v>61</v>
       </c>
       <c r="AU5" t="str">
-        <v/>
+        <v>year</v>
       </c>
       <c r="AV5" t="str">
         <v>60 - 69</v>
@@ -1890,7 +1890,7 @@
         <v>2020-01-10</v>
       </c>
       <c r="BA5" t="str">
-        <v>Dyspnea (breathing difficulty); Malaise (general discomfort/unease); Rhinorrhea (runny nose); Tachypnea (accelerated respiratory rate); Vomiting (throwing up)</v>
+        <v>Coma; Dyspnea (breathing difficulty); Rhinorrhea (runny nose)</v>
       </c>
       <c r="BB5" t="str">
         <v>Anemia</v>
@@ -1905,7 +1905,7 @@
         <v>Dublin</v>
       </c>
       <c r="BF5" t="str">
-        <v>Dublin Region</v>
+        <v>Dublin</v>
       </c>
       <c r="BG5" t="str">
         <v>Ireland</v>
@@ -1920,7 +1920,7 @@
         <v>Canada, New Brunswick</v>
       </c>
       <c r="BK5" t="str">
-        <v>Other</v>
+        <v>Missing</v>
       </c>
       <c r="BL5" t="str">
         <v>Direct</v>
@@ -2189,10 +2189,10 @@
         <v>mRNA (cDNA)</v>
       </c>
       <c r="AN6" t="str">
-        <v>Pig</v>
+        <v>Human</v>
       </c>
       <c r="AO6" t="str">
-        <v>Sus scrofa domesticus</v>
+        <v>Homo sapiens</v>
       </c>
       <c r="AP6" t="str">
         <v>Not Applicable</v>
@@ -2210,7 +2210,7 @@
         <v>84</v>
       </c>
       <c r="AU6" t="str">
-        <v/>
+        <v>year</v>
       </c>
       <c r="AV6" t="str">
         <v>80 - 89</v>
@@ -2228,7 +2228,7 @@
         <v>2020-02-22</v>
       </c>
       <c r="BA6" t="str">
-        <v>Confusion; Irritability; Asthenia (general weakness); Cough</v>
+        <v>Confusion; Irritability; Cough</v>
       </c>
       <c r="BB6" t="str">
         <v>Hypertension (high blood pressure); Postpartum (≤6 weeks)</v>
@@ -2243,7 +2243,7 @@
         <v>Nice</v>
       </c>
       <c r="BF6" t="str">
-        <v>Provence-Alpes-Cote d'Azur Region</v>
+        <v>Provence-Alpes-Cote d'Azur</v>
       </c>
       <c r="BG6" t="str">
         <v>France</v>
@@ -2548,7 +2548,7 @@
         <v>86</v>
       </c>
       <c r="AU7" t="str">
-        <v/>
+        <v>year</v>
       </c>
       <c r="AV7" t="str">
         <v>80 - 89</v>
@@ -2566,7 +2566,7 @@
         <v>2020-02-13</v>
       </c>
       <c r="BA7" t="str">
-        <v>Parageusia (distorted sense of taste); Nonproductive cough (dry cough); Dyspnea (breathing difficulty); Encephalitis (brain inflammation); Fever (≥38°C)</v>
+        <v>Cognitive impairment; Fever</v>
       </c>
       <c r="BB7" t="str">
         <v>Lupus; Sickle cell disease</v>
@@ -2578,7 +2578,7 @@
         <v>Johannesberg</v>
       </c>
       <c r="BF7" t="str">
-        <v>Gauteng Province</v>
+        <v>Gauteng</v>
       </c>
       <c r="BG7" t="str">
         <v>South Africa</v>

</xml_diff>